<commit_message>
Defect report and evidence files
</commit_message>
<xml_diff>
--- a/docs/Defects - TodoLy.xlsx
+++ b/docs/Defects - TodoLy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t xml:space="preserve">Bug ID</t>
   </si>
@@ -67,18 +67,87 @@
     <t xml:space="preserve">This issue is can be caused by improper exception/error handling.</t>
   </si>
   <si>
-    <t xml:space="preserve">No generic 500 server error. Custom error handling with specific error messages.</t>
+    <t xml:space="preserve">n/a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Make a request with an invalid payload. </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">i.e. put "&lt;&lt;" characters in the body</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">No generic 500 server error. Correct error handling with specific error messages.</t>
   </si>
   <si>
     <t xml:space="preserve">A generic “Server Error” page is displayed in html format.</t>
   </si>
   <si>
-    <t xml:space="preserve">createUserInvalidPayloadTest</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">createUserInvalidPayloadTest
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CreateUserWithInvalidAddItemMoreExpanded</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Medium</t>
   </si>
   <si>
+    <t xml:space="preserve">BUG_001_generic_server_error.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diego Bruno</t>
   </si>
   <si>
@@ -89,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">No json format in response body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Make a json request to the isAuthenticated API method.</t>
   </si>
   <si>
     <t xml:space="preserve">" A JSON payload should start with an openning curly brace '{' or an openning square bracket '['. "</t>
@@ -105,19 +177,32 @@
     <t xml:space="preserve">High</t>
   </si>
   <si>
+    <t xml:space="preserve">BUG_002_No_valid_json_format_in_isAuthenticated_response.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUG_003</t>
   </si>
   <si>
     <t xml:space="preserve">User can be created with invalid values </t>
   </si>
   <si>
-    <t xml:space="preserve">This issue only describes one of many ways of creating an invalid user object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High impact: makes UI access impossible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">createUserWithInvalidAddItemMoreExpanded</t>
+    <t xml:space="preserve">CreateUser can be called with invalid values in a way that will prevent the user from accessing the UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Make a request to the CreateUser method and include a value  for DefaultProjectId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CreateUser should not allow for some values to be passed in the request. DefaultProjectId should always be auto-generated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserObject is created with an invalid state.
+High impact: makes UI access impossible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createUserWithDefaultProjectId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUG_003_User can be created with invalid value and locked out of UI.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">BUG_004</t>
@@ -126,28 +211,53 @@
     <t xml:space="preserve">Create user: wrong message on email format validation: @mail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">The error message does not match with the scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Make a request to the CreateUSer method with an email in the format "@xxxx.xxx"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Email Address error code 307 should be displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Input Data error code 302 is displayed</t>
+  </si>
+  <si>
     <t xml:space="preserve">TODO: not automated</t>
   </si>
   <si>
     <t xml:space="preserve">Low</t>
   </si>
   <si>
+    <t xml:space="preserve">BUG_004_Incorrect_email_format_error_message.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">BUG_005</t>
   </si>
   <si>
-    <t xml:space="preserve">Update user: no email format validation: @mail.com</t>
+    <t xml:space="preserve">Update user: incorrect format validation: @mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">User is able to change the email to a invalid format.</t>
   </si>
   <si>
-    <t xml:space="preserve">Validation of email format in User Update functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No validation for certain email formats. Allows the user to have a “@mail.com” email address</t>
+    <t xml:space="preserve">Existing valid user account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Authenticate with valid user (get token)
+- Make a Update User call and change the email value to a format “@xxxx.xxx”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation of email format in User Update functionality should not allow invalid email format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No validation for certain email formats. Allows the user to have a “@xxxx.xxx email address</t>
   </si>
   <si>
     <t xml:space="preserve">updateInValidEmailTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUG_005_incorrect email format validation in user update.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">BUG_006</t>
@@ -179,7 +289,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,9 +323,15 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -285,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +423,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,7 +516,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -449,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -459,160 +579,198 @@
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="K2" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="J6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>41</v>
+      <c r="A7" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Updated evidence file and documentation
</commit_message>
<xml_diff>
--- a/docs/Defects - TodoLy.xlsx
+++ b/docs/Defects - TodoLy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t xml:space="preserve">Bug ID</t>
   </si>
@@ -269,7 +269,20 @@
     <t xml:space="preserve">This is a critical security issue because it allows for unauthorized deletion of a project that belongs to another user.</t>
   </si>
   <si>
-    <t xml:space="preserve">User should not be able to be created with arbitrary DefaultProjectId</t>
+    <t xml:space="preserve">BUG_003 has not been fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Create a user_A and note its defaultProjectId
+- Use user_A credentials to make a request to GetAllProjects to verify that it the defaultProjectId is present
+- Optional: login to the UI to see the project being there
+- Create a user_B and force it to have a defaultProjectId with the same value as the defaultProjectId that user_A has (exploiting BUG_003 from this document)
+- Use user_B credentials to make a request to "Delete a Project By Id" against the id of user_A defaultProjectId
+- One more time use user_A credentials and make a request to GetAllProjects to verify the status of projects. Notice that the value defaultProjectId is missing
+- Optional: refresh the UI to see how user_A project has been deleted by the user_B request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to be created with arbitrary DefaultProjectId.
+This is an exploit of BUG_003 as reported in this document.</t>
   </si>
   <si>
     <t xml:space="preserve">CRITICAL impact: Allows deletion of any project without permission from the owner.</t>
@@ -280,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">CRITICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUG_006_User can delete projects fom other users.mp4</t>
   </si>
 </sst>
 </file>
@@ -355,8 +371,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEF413D"/>
-        <bgColor rgb="FF993366"/>
+        <fgColor rgb="FFF58220"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -489,8 +505,8 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF9BBB59"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFEF413D"/>
+      <rgbColor rgb="FFF58220"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -516,7 +532,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -524,8 +540,8 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="33.76"/>
@@ -744,32 +760,38 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="F7" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="G7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="I7" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>